<commit_message>
Added Celsee part numbers.
</commit_message>
<xml_diff>
--- a/BOM - Gronk/GronkDaughter-BOM.xlsx
+++ b/BOM - Gronk/GronkDaughter-BOM.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boniface\Documents\GitHub\PCB\Projects\PREP400\BOM - Gronk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A9348D-E238-4787-8D8F-E64454A7098F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318B3189-6A83-4CF1-8F2C-EDDA19100416}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="4548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backflow" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="276">
   <si>
     <t>U1</t>
   </si>
@@ -848,6 +855,9 @@
   </si>
   <si>
     <t>D31, D32, D35, D36, D37, D38, D39, D40</t>
+  </si>
+  <si>
+    <t>CelseePartNum</t>
   </si>
 </sst>
 </file>
@@ -1475,6 +1485,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1486,9 +1499,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1811,1600 +1821,1756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:A75"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>16000004</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="16">
+      <c r="C2" s="16">
         <v>40</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="24">
+      <c r="C3" s="24">
         <v>44</v>
       </c>
-      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="I3" s="30"/>
-    </row>
-    <row r="4" spans="1:9" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="J3" s="26"/>
+    </row>
+    <row r="4" spans="1:10" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B4" s="16">
+      <c r="C4" s="16">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>16000068</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="16">
+      <c r="C5" s="16">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="B6" s="24">
+      <c r="C6" s="24">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="25" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>16000069</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="B7" s="16">
+      <c r="C7" s="16">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="H7" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="24" t="s">
         <v>257</v>
       </c>
-      <c r="B8" s="24">
+      <c r="C8" s="24">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>16000070</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="16">
+      <c r="C9" s="16">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="B10" s="24">
+      <c r="C10" s="24">
         <v>4</v>
       </c>
-      <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="25" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>16000071</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="B11" s="16">
+      <c r="C11" s="16">
         <v>4</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="G11" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="B12" s="24">
+      <c r="C12" s="24">
         <v>5</v>
       </c>
-      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="16">
+      <c r="C13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:10" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>16000072</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="B14" s="16">
+      <c r="C14" s="16">
         <v>36</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="B15" s="24">
+      <c r="C15" s="24">
         <v>41</v>
       </c>
-      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="25" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="B16" s="16">
+      <c r="C16" s="16">
         <v>1</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="6"/>
+      <c r="I16" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="16">
+      <c r="C17" s="16">
         <v>1</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>16000094</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B18" s="16">
+      <c r="C18" s="16">
         <v>2</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="G18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="B19" s="24">
+      <c r="C19" s="24">
         <v>2</v>
       </c>
-      <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="25" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>16000073</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B20" s="16">
+      <c r="C20" s="16">
         <v>2</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="G20" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="B21" s="24">
+      <c r="C21" s="24">
         <v>2</v>
       </c>
-      <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="25" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>16000074</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="16">
+      <c r="C22" s="16">
         <v>6</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>16000056</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="B23" s="16">
+      <c r="C23" s="16">
         <v>6</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="B24" s="24">
+      <c r="C24" s="24">
         <v>2</v>
       </c>
-      <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="25" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>16000075</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="B25" s="16">
+      <c r="C25" s="16">
         <v>4</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
+      <c r="H25" s="6"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="B26" s="24">
+      <c r="C26" s="24">
         <v>4</v>
       </c>
-      <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="25" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>16000095</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="B27" s="16">
+      <c r="C27" s="16">
         <v>8</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="B28" s="24">
+      <c r="C28" s="24">
         <v>4</v>
       </c>
-      <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="25" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>16000098</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B29" s="16">
+      <c r="C29" s="16">
         <v>2</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
+      <c r="H29" s="6"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="B30" s="24">
+      <c r="C30" s="24">
         <v>2</v>
       </c>
-      <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="25" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="6">
+        <v>16000020</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>266</v>
       </c>
-      <c r="B31" s="16">
+      <c r="C31" s="16">
         <v>4</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="B32" s="24">
+      <c r="C32" s="24">
         <v>4</v>
       </c>
-      <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="25" t="s">
+      <c r="E32" s="6"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>16000076</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B33" s="16">
+      <c r="C33" s="16">
         <v>1</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="F33" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="G33" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="B34" s="24">
+      <c r="C34" s="24">
         <v>1</v>
       </c>
-      <c r="C34" s="6"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="25" t="s">
+      <c r="E34" s="6"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="B35" s="16">
+      <c r="C35" s="16">
         <v>1</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="F35" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="16" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>16000021</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="B36" s="16">
+      <c r="C36" s="16">
         <v>7</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="G36" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="B37" s="24">
+      <c r="C37" s="24">
         <v>1</v>
       </c>
-      <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="25" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="16" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="6">
+        <v>16000022</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B38" s="16">
+      <c r="C38" s="16">
         <v>6</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="B39" s="24">
+      <c r="C39" s="24">
         <v>2</v>
       </c>
-      <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="25" t="s">
+      <c r="E39" s="6"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>16000023</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="B40" s="16">
+      <c r="C40" s="16">
         <v>4</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="G40" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="B41" s="24">
+      <c r="C41" s="24">
         <v>4</v>
       </c>
-      <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="25" t="s">
+      <c r="E41" s="6"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="16" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>16000077</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B42" s="16">
+      <c r="C42" s="16">
         <v>2</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="F42" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="G42" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="H42" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="22" t="s">
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B43" s="24">
+      <c r="C43" s="24">
         <v>2</v>
       </c>
-      <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="25" t="s">
+      <c r="E43" s="6"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>16000078</v>
+      </c>
+      <c r="B44" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="B44" s="16">
+      <c r="C44" s="16">
         <v>6</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="F44" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="G44" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="I44" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="27"/>
-      <c r="B45" s="16">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>16000079</v>
+      </c>
+      <c r="B45" s="28"/>
+      <c r="C45" s="16">
         <v>6</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="H45" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="23" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="B46" s="24">
+      <c r="C46" s="24">
         <v>6</v>
       </c>
-      <c r="C46" s="6"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="8"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="9"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="8"/>
+      <c r="I46" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B47" s="16">
+      <c r="C47" s="16">
         <v>1</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="F47" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="G47" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="I47" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="16" t="s">
+    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B48" s="16">
+      <c r="C48" s="16">
         <v>11</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="F48" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="G48" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="H48" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="5" t="s">
+      <c r="I48" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>16000080</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="16">
+      <c r="C49" s="16">
         <v>1</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="F49" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="G49" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="21"/>
+      <c r="I49" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="16" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="6">
+        <v>16000081</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B50" s="16">
+      <c r="C50" s="16">
         <v>6</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="G50" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="24" t="s">
+      <c r="H50" s="6"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="B51" s="24">
+      <c r="C51" s="24">
         <v>1</v>
       </c>
-      <c r="C51" s="6"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="25" t="s">
+      <c r="E51" s="6"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="16" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>16000082</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B52" s="16">
+      <c r="C52" s="16">
         <v>6</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="F52" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="G52" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="H52" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="B53" s="24">
+      <c r="C53" s="24">
         <v>1</v>
       </c>
-      <c r="C53" s="6"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="25" t="s">
+      <c r="E53" s="6"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="16" t="s">
+    <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>16000083</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="B54" s="16">
+      <c r="C54" s="16">
         <v>9</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="F54" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="6"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="24" t="s">
+      <c r="H54" s="20"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="B55" s="24">
+      <c r="C55" s="24">
         <v>4</v>
       </c>
-      <c r="C55" s="8"/>
       <c r="D55" s="8"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="25" t="s">
+      <c r="E55" s="8"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16" t="s">
+    <row r="56" spans="1:9" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6">
+        <v>16000096</v>
+      </c>
+      <c r="B56" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B56" s="16">
+      <c r="C56" s="16">
         <v>16</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="F56" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="G56" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="G56" s="6"/>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24" t="s">
+      <c r="H56" s="6"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="B57" s="24">
+      <c r="C57" s="24">
         <v>8</v>
       </c>
-      <c r="C57" s="8"/>
       <c r="D57" s="8"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="25" t="s">
+      <c r="E57" s="8"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="6">
+        <v>16000097</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B58" s="16">
+      <c r="C58" s="16">
         <v>2</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="D58" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="F58" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="G58" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="H58" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="24" t="s">
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="B59" s="24">
+      <c r="C59" s="24">
         <v>2</v>
       </c>
-      <c r="C59" s="8"/>
       <c r="D59" s="8"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="25" t="s">
+      <c r="E59" s="8"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="16" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
+        <v>16000084</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="B60" s="16">
+      <c r="C60" s="16">
         <v>6</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="D60" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="F60" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="G60" s="6"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="24" t="s">
+      <c r="H60" s="6"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="6"/>
+      <c r="B61" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="B61" s="24">
+      <c r="C61" s="24">
         <v>6</v>
       </c>
-      <c r="C61" s="8"/>
       <c r="D61" s="8"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="25" t="s">
+      <c r="E61" s="8"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="16" t="s">
+    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="6">
+        <v>16000037</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="B62" s="16">
+      <c r="C62" s="16">
         <v>8</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="D62" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="F62" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="G62" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="24" t="s">
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="6"/>
+      <c r="B63" s="24" t="s">
         <v>245</v>
       </c>
-      <c r="B63" s="24">
+      <c r="C63" s="24">
         <v>4</v>
       </c>
-      <c r="C63" s="8"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25" t="s">
+      <c r="E63" s="8"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="25"/>
+      <c r="I63" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="16" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="6">
+        <v>16000085</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="B64" s="16">
+      <c r="C64" s="16">
         <v>1</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E64" s="13" t="s">
+      <c r="F64" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="20" t="s">
+      <c r="G64" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G64" s="6"/>
-      <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="24" t="s">
+      <c r="H64" s="6"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="6"/>
+      <c r="B65" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="B65" s="24">
+      <c r="C65" s="24">
         <v>1</v>
       </c>
-      <c r="C65" s="8"/>
       <c r="D65" s="8"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="25" t="s">
+      <c r="E65" s="8"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="25" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="16" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="6">
+        <v>16000060</v>
+      </c>
+      <c r="B66" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="16">
+      <c r="C66" s="16">
         <v>2</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="D66" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="13" t="s">
+      <c r="F66" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="G66" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G66" s="6" t="s">
+      <c r="H66" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16" t="s">
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+      <c r="B67" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B67" s="16">
+      <c r="C67" s="16">
         <v>52</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="D67" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="E67" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="F67" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="G67" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G67" s="8" t="s">
+      <c r="H67" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="I67" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="17" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="6">
+        <v>16000086</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B68" s="19">
+      <c r="C68" s="19">
         <v>4</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="D68" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="E68" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="F68" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="G68" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G68" s="6" t="s">
+      <c r="H68" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="28" t="s">
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="6">
+        <v>16000087</v>
+      </c>
+      <c r="B69" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="16">
+      <c r="C69" s="16">
         <v>1</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="D69" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="E69" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E69" s="9" t="s">
+      <c r="F69" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="G69" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G69" s="6" t="s">
+      <c r="H69" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="I69" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="28"/>
-      <c r="B70" s="16">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="6">
+        <v>16000088</v>
+      </c>
+      <c r="B70" s="29"/>
+      <c r="C70" s="16">
         <v>2</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="D70" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="E70" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="F70" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="G70" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="H70" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="I70" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="28"/>
-      <c r="B71" s="16">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="6">
+        <v>16000089</v>
+      </c>
+      <c r="B71" s="29"/>
+      <c r="C71" s="16">
         <v>1</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="D71" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="E71" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="6" t="s">
+      <c r="G71" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="H71" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="I71" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="29"/>
-      <c r="B72" s="16">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="6">
+        <v>16000090</v>
+      </c>
+      <c r="B72" s="30"/>
+      <c r="C72" s="16">
         <v>1</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="F72" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F72" s="6" t="s">
+      <c r="G72" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="5" t="s">
+      <c r="H72" s="6"/>
+      <c r="I72" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="29"/>
-      <c r="B73" s="16">
+    <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="6">
+        <v>16000091</v>
+      </c>
+      <c r="B73" s="30"/>
+      <c r="C73" s="16">
         <v>1</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="E73" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="G73" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="H73" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="I73" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="29"/>
-      <c r="B74" s="16">
+    <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A74" s="6">
+        <v>16000092</v>
+      </c>
+      <c r="B74" s="30"/>
+      <c r="C74" s="16">
         <v>2</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="D74" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="E74" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="F74" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="G74" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="H74" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="I74" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="29"/>
-      <c r="B75" s="16">
+    <row r="75" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="6">
+        <v>16000093</v>
+      </c>
+      <c r="B75" s="30"/>
+      <c r="C75" s="16">
         <v>1</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="D75" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="E75" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="F75" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="G75" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G75" s="5" t="s">
+      <c r="H75" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="I75" s="5" t="s">
         <v>159</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B69:B75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>